<commit_message>
Dodaj nowe podzadanie do meta macierzy odpowiedzialności ćwiczenia 3
</commit_message>
<xml_diff>
--- a/cwiczenie-3-meta/macierz-odpowiedzialnosci/figury/macierz-odpowiedzialnosci.xlsx
+++ b/cwiczenie-3-meta/macierz-odpowiedzialnosci/figury/macierz-odpowiedzialnosci.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="1220" windowWidth="23240" windowHeight="17260"/>
+    <workbookView xWindow="7080" yWindow="1220" windowWidth="23240" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$17</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" dpi="72" codePage="65001"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
   <si>
     <t>R</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Testowanie</t>
   </si>
   <si>
-    <t>Organizacja środowiska pracy</t>
-  </si>
-  <si>
     <t>Tomasz
 Cudziło</t>
   </si>
@@ -124,6 +121,12 @@
   <si>
     <t>Michał
 Słotwiński</t>
+  </si>
+  <si>
+    <t>Koordynacja pracy</t>
+  </si>
+  <si>
+    <t>Administracja infrastruktury</t>
   </si>
 </sst>
 </file>
@@ -228,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -313,11 +316,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -423,6 +435,18 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -438,8 +462,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFA8F"/>
       <color rgb="FF7CBF33"/>
-      <color rgb="FFFFFA8F"/>
       <color rgb="FFEFA5A3"/>
       <color rgb="FFF6D900"/>
       <color rgb="FFE1514D"/>
@@ -748,10 +772,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I16"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -766,25 +790,25 @@
       <c r="A1" s="35"/>
       <c r="B1" s="35"/>
       <c r="C1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="I1" s="22" t="s">
         <v>22</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1">
@@ -931,7 +955,7 @@
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="29" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="7" t="s">
@@ -951,125 +975,146 @@
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
-      <c r="A11" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="7" t="s">
+      <c r="A11" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="37"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
-      <c r="A12" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="10" t="s">
+      <c r="A12" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="10"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
-      <c r="A13" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="13" t="s">
+      <c r="A13" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="34"/>
+      <c r="C13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="10"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
-      <c r="A14" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="19" t="s">
+      <c r="A14" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="A15" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="31"/>
+      <c r="C15" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="90" customHeight="1">
-      <c r="A16" s="36" t="s">
+    <row r="16" spans="1:12" ht="30" customHeight="1">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" ht="90" customHeight="1">
+      <c r="A17" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A17:I17"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="89" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="1.1811023622047245" right="1.1811023622047245" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="84" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>